<commit_message>
Making changes to tech4 list and downloaded zip
</commit_message>
<xml_diff>
--- a/Placement_file/Placement_file.xlsx
+++ b/Placement_file/Placement_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Position</t>
   </si>
@@ -353,6 +353,51 @@
   </si>
   <si>
     <t>U7-3</t>
+  </si>
+  <si>
+    <t>U7-4</t>
+  </si>
+  <si>
+    <t>U7-5</t>
+  </si>
+  <si>
+    <t>U7-6</t>
+  </si>
+  <si>
+    <t>U7-7</t>
+  </si>
+  <si>
+    <t>U7-8</t>
+  </si>
+  <si>
+    <t>U7-9</t>
+  </si>
+  <si>
+    <t>U7-10</t>
+  </si>
+  <si>
+    <t>U7-11</t>
+  </si>
+  <si>
+    <t>U7-12</t>
+  </si>
+  <si>
+    <t>U7-13</t>
+  </si>
+  <si>
+    <t>U7-14</t>
+  </si>
+  <si>
+    <t>U7-15</t>
+  </si>
+  <si>
+    <t>U7-16</t>
+  </si>
+  <si>
+    <t>U7-17</t>
+  </si>
+  <si>
+    <t>U7-18</t>
   </si>
 </sst>
 </file>
@@ -684,7 +729,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -703,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>516</v>
+        <v>856</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -711,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>579</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -719,7 +764,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>796</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -727,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>805</v>
+        <v>579</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -735,7 +780,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>807</v>
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -743,7 +788,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>829</v>
+        <v>767</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -751,7 +796,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>851</v>
+        <v>805</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -759,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>517</v>
+        <v>806</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -767,7 +812,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>536</v>
+        <v>807</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -775,7 +820,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>544</v>
+        <v>829</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -783,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>547</v>
+        <v>513</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -791,7 +836,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>557</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -799,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>569</v>
+        <v>534</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -807,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>591</v>
+        <v>535</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -815,7 +860,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>592</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -823,7 +868,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>600</v>
+        <v>547</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -831,7 +876,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>611</v>
+        <v>551</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -839,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>646</v>
+        <v>569</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -847,7 +892,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>647</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -855,7 +900,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>649</v>
+        <v>591</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -863,7 +908,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>650</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -871,7 +916,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>654</v>
+        <v>600</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -879,7 +924,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>655</v>
+        <v>611</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -887,7 +932,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>659</v>
+        <v>646</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -895,7 +940,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>661</v>
+        <v>647</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -903,7 +948,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>662</v>
+        <v>649</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -911,7 +956,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>671</v>
+        <v>650</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -919,7 +964,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>677</v>
+        <v>653</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -927,7 +972,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>682</v>
+        <v>654</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -935,7 +980,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>684</v>
+        <v>655</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -943,7 +988,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>705</v>
+        <v>661</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -951,7 +996,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>706</v>
+        <v>662</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -959,7 +1004,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>709</v>
+        <v>677</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -967,7 +1012,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>715</v>
+        <v>705</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -975,7 +1020,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>718</v>
+        <v>706</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -983,7 +1028,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>720</v>
+        <v>709</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -991,7 +1036,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>727</v>
+        <v>715</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -999,7 +1044,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>730</v>
+        <v>719</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1007,7 +1052,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>733</v>
+        <v>720</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1015,7 +1060,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1023,7 +1068,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>737</v>
+        <v>730</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1031,7 +1076,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>738</v>
+        <v>733</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1039,7 +1084,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>743</v>
+        <v>734</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1047,7 +1092,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>744</v>
+        <v>735</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1055,7 +1100,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>748</v>
+        <v>737</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1063,7 +1108,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>753</v>
+        <v>742</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1071,7 +1116,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>756</v>
+        <v>743</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1079,7 +1124,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>758</v>
+        <v>744</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1087,7 +1132,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>763</v>
+        <v>748</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1095,7 +1140,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>768</v>
+        <v>753</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1103,7 +1148,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>770</v>
+        <v>756</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1111,7 +1156,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>772</v>
+        <v>758</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1119,7 +1164,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>774</v>
+        <v>760</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1127,7 +1172,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>775</v>
+        <v>763</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1135,7 +1180,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>782</v>
+        <v>768</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1143,7 +1188,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>787</v>
+        <v>770</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1151,7 +1196,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>795</v>
+        <v>771</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1159,7 +1204,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>797</v>
+        <v>772</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1167,7 +1212,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>798</v>
+        <v>774</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1175,7 +1220,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>810</v>
+        <v>775</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1183,7 +1228,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>820</v>
+        <v>787</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1191,7 +1236,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>821</v>
+        <v>797</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1199,7 +1244,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>822</v>
+        <v>798</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1207,7 +1252,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>823</v>
+        <v>813</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1215,7 +1260,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>831</v>
+        <v>821</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1223,7 +1268,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>832</v>
+        <v>822</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1231,7 +1276,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>835</v>
+        <v>823</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1239,7 +1284,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>839</v>
+        <v>831</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1247,7 +1292,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>841</v>
+        <v>832</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1255,7 +1300,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>844</v>
+        <v>839</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1263,7 +1308,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>848</v>
+        <v>843</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1271,7 +1316,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>853</v>
+        <v>844</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1279,7 +1324,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>510</v>
+        <v>848</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1287,7 +1332,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>581</v>
+        <v>849</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1295,7 +1340,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>582</v>
+        <v>853</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1303,7 +1348,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>587</v>
+        <v>510</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1311,7 +1356,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>612</v>
+        <v>574</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1319,7 +1364,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>651</v>
+        <v>576</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1327,7 +1372,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>675</v>
+        <v>581</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1335,7 +1380,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>686</v>
+        <v>583</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1343,7 +1388,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>687</v>
+        <v>651</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1351,7 +1396,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>700</v>
+        <v>671</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1359,7 +1404,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>713</v>
+        <v>675</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1367,7 +1412,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>716</v>
+        <v>686</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1375,7 +1420,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>739</v>
+        <v>687</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1383,7 +1428,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>747</v>
+        <v>713</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1391,7 +1436,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>749</v>
+        <v>716</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1399,7 +1444,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>751</v>
+        <v>718</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1407,7 +1452,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>752</v>
+        <v>728</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1415,7 +1460,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>754</v>
+        <v>739</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1423,7 +1468,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>762</v>
+        <v>747</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1431,7 +1476,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>777</v>
+        <v>749</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1439,7 +1484,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>784</v>
+        <v>750</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1447,7 +1492,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>790</v>
+        <v>751</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1455,7 +1500,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>793</v>
+        <v>752</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1463,7 +1508,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>801</v>
+        <v>754</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1471,7 +1516,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>802</v>
+        <v>762</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1479,7 +1524,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>803</v>
+        <v>769</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1487,7 +1532,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>809</v>
+        <v>773</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1495,7 +1540,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>834</v>
+        <v>777</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1503,7 +1548,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>843</v>
+        <v>784</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1511,7 +1556,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>512</v>
+        <v>790</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1519,7 +1564,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>603</v>
+        <v>791</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1527,7 +1572,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>683</v>
+        <v>793</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1535,7 +1580,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>750</v>
+        <v>796</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1543,7 +1588,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>764</v>
+        <v>801</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1551,7 +1596,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>773</v>
+        <v>803</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1559,7 +1604,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>779</v>
+        <v>809</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1567,7 +1612,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>828</v>
+        <v>810</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1575,7 +1620,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1583,7 +1628,127 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>583</v>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127">
+        <v>660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>